<commit_message>
Moving figures into place
</commit_message>
<xml_diff>
--- a/latex/performance_content/scaling/ItascaWeakScaling.xlsx
+++ b/latex/performance_content/scaling/ItascaWeakScaling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="14500" tabRatio="500" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="1420" yWindow="0" windowWidth="25120" windowHeight="14920" tabRatio="500" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="n50_weak_alltoallv" sheetId="6" r:id="rId1"/>
@@ -325,28 +325,74 @@
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
-              <a:defRPr sz="2000"/>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2000"/>
-              <a:t>Weak Scaling </a:t>
+              <a:t>Weak Scaling,</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Np = 4000 points</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2000"/>
           </a:p>
           <a:p>
-            <a:pPr>
-              <a:defRPr sz="2000"/>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2000"/>
               <a:t>SpMV + MPI (Isend/Irecv Overlap CPU) on Itasca </a:t>
-            </a:r>
-            <a:br>
-              <a:rPr lang="en-US" sz="2000"/>
-            </a:br>
-            <a:r>
-              <a:rPr lang="en-US" sz="2000"/>
-              <a:t>Np = 4000 points</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -854,28 +900,74 @@
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
-              <a:defRPr sz="2000"/>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2000"/>
-              <a:t>Weak Scaling Efficiency </a:t>
+              <a:t>Weak Scaling Efficiency,</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Np = 4000 points</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2000"/>
           </a:p>
           <a:p>
-            <a:pPr>
-              <a:defRPr sz="2000"/>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2000"/>
               <a:t>SpMV + MPI (Isend/Irecv Overlap CPU) on Itasca </a:t>
-            </a:r>
-            <a:br>
-              <a:rPr lang="en-US" sz="2000"/>
-            </a:br>
-            <a:r>
-              <a:rPr lang="en-US" sz="2000"/>
-              <a:t>Np = 4000 points</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1320,7 +1412,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Efficiency</a:t>
+                  <a:t>Efficiency (t_1/t_p)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1384,28 +1476,70 @@
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
-              <a:defRPr sz="2000"/>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2000"/>
-              <a:t>Weak Scaling Comparison</a:t>
+              <a:t>Weak Scaling Comparison, </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Np = 4000 points</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2000"/>
           </a:p>
           <a:p>
-            <a:pPr>
-              <a:defRPr sz="2000"/>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2000"/>
               <a:t>SpMV + MPI on Itasca </a:t>
-            </a:r>
-            <a:br>
-              <a:rPr lang="en-US" sz="2000"/>
-            </a:br>
-            <a:r>
-              <a:rPr lang="en-US" sz="2000"/>
-              <a:t>Np = 4000 points</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2837,7 +2971,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3690,7 +3824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A38" sqref="A38:C38"/>
     </sheetView>
   </sheetViews>
@@ -4717,7 +4851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -6219,8 +6353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>